<commit_message>
Load modules for youtube and imdb datasets, mat files conversions
</commit_message>
<xml_diff>
--- a/data/european-celebrities/european-celebs.xlsx
+++ b/data/european-celebrities/european-celebs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\telemachos\Documents\Programming\python\projects\Face-Recognition\data\european-celebrities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B427C2-1A63-490C-8950-F9378AB951AA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF59C9ED-1D60-4E9D-B596-CF65637F6092}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10704" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{1EE1D400-50AF-4419-A32E-91D79DFE8ADC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Name</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Harry Styles</t>
+  </si>
+  <si>
+    <t>data/european-celebrities/train/connor_mcgregor</t>
+  </si>
+  <si>
+    <t>data/european-celebrities/val/connor_mcgregor</t>
+  </si>
+  <si>
+    <t>data/european-celebrities/train/adele</t>
+  </si>
+  <si>
+    <t>data/european-celebrities/val/adele</t>
   </si>
 </sst>
 </file>
@@ -526,7 +538,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,6 +633,12 @@
       <c r="D5">
         <v>6</v>
       </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -682,6 +700,12 @@
       </c>
       <c r="D12">
         <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>